<commit_message>
Adding working clustering website, adding feature of loading previous graph, create a subgraph from a gene
</commit_message>
<xml_diff>
--- a/database/Demo #2_ Weighted GRN (15 genes, 28 edges, Dahlquist Lab unpublished data).xlsx
+++ b/database/Demo #2_ Weighted GRN (15 genes, 28 edges, Dahlquist Lab unpublished data).xlsx
@@ -1,19 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maikatran/Research/graph-research/graph-nextjs/database/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF88382-2B47-D746-9107-A130003CF169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="network" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+  <si>
+    <t>cols regulators/rows targets</t>
+  </si>
+  <si>
+    <t>ACE2</t>
+  </si>
+  <si>
+    <t>ASH1</t>
+  </si>
+  <si>
+    <t>CIN5</t>
+  </si>
+  <si>
+    <t>GCR2</t>
+  </si>
+  <si>
+    <t>GLN3</t>
+  </si>
+  <si>
+    <t>HAP4</t>
+  </si>
+  <si>
+    <t>HMO1</t>
+  </si>
+  <si>
+    <t>MSN2</t>
+  </si>
+  <si>
+    <t>SFP1</t>
+  </si>
+  <si>
+    <t>STB5</t>
+  </si>
+  <si>
+    <t>SWI4</t>
+  </si>
+  <si>
+    <t>SWI5</t>
+  </si>
+  <si>
+    <t>YHP1</t>
+  </si>
+  <si>
+    <t>YOX1</t>
+  </si>
+  <si>
+    <t>ZAP1</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -43,13 +104,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -374,62 +443,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>cols regulators/rows targets</v>
-      </c>
-      <c r="B1" t="str">
-        <v>ACE2</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ASH1</v>
-      </c>
-      <c r="D1" t="str">
-        <v>CIN5</v>
-      </c>
-      <c r="E1" t="str">
-        <v>GCR2</v>
-      </c>
-      <c r="F1" t="str">
-        <v>GLN3</v>
-      </c>
-      <c r="G1" t="str">
-        <v>HAP4</v>
-      </c>
-      <c r="H1" t="str">
-        <v>HMO1</v>
-      </c>
-      <c r="I1" t="str">
-        <v>MSN2</v>
-      </c>
-      <c r="J1" t="str">
-        <v>SFP1</v>
-      </c>
-      <c r="K1" t="str">
-        <v>STB5</v>
-      </c>
-      <c r="L1" t="str">
-        <v>SWI4</v>
-      </c>
-      <c r="M1" t="str">
-        <v>SWI5</v>
-      </c>
-      <c r="N1" t="str">
-        <v>YHP1</v>
-      </c>
-      <c r="O1" t="str">
-        <v>YOX1</v>
-      </c>
-      <c r="P1" t="str">
-        <v>ZAP1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>ACE2</v>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -477,9 +555,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>ASH1</v>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -527,9 +605,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>CIN5</v>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -577,9 +655,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>GCR2</v>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -627,9 +705,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>GLN3</v>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -677,9 +755,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>HAP4</v>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -727,9 +805,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>HMO1</v>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -777,9 +855,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>MSN2</v>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -827,9 +905,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>SFP1</v>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -877,9 +955,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>STB5</v>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -927,9 +1005,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>SWI4</v>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -977,9 +1055,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>SWI5</v>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1027,9 +1105,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>YHP1</v>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1077,9 +1155,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>YOX1</v>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1127,9 +1205,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>ZAP1</v>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1178,5 +1256,6 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>